<commit_message>
Made changes on create ticket
</commit_message>
<xml_diff>
--- a/Attachments/Testing.xlsx
+++ b/Attachments/Testing.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Ticket Type</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Penina Waithaka</t>
+  </si>
+  <si>
+    <t>Login</t>
   </si>
 </sst>
 </file>
@@ -378,7 +381,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -428,6 +431,9 @@
       <c r="A3" t="s">
         <v>9</v>
       </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>

</xml_diff>